<commit_message>
adjust the excel export output -bold the column title
</commit_message>
<xml_diff>
--- a/teacher_list.xlsx
+++ b/teacher_list.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Employer ID</t>
   </si>
@@ -29,6 +29,27 @@
     <t>Borrowed Books</t>
   </si>
   <si>
+    <t>424343242</t>
+  </si>
+  <si>
+    <t>Killua</t>
+  </si>
+  <si>
+    <t>CHK</t>
+  </si>
+  <si>
+    <t>9087742344</t>
+  </si>
+  <si>
+    <t>989883234</t>
+  </si>
+  <si>
+    <t>Reeka</t>
+  </si>
+  <si>
+    <t>09876543883</t>
+  </si>
+  <si>
     <t>a1212311321</t>
   </si>
   <si>
@@ -48,6 +69,15 @@
   </si>
   <si>
     <t>098765432</t>
+  </si>
+  <si>
+    <t>p98124233</t>
+  </si>
+  <si>
+    <t>Killjoy</t>
+  </si>
+  <si>
+    <t>097783213412</t>
   </si>
 </sst>
 </file>
@@ -55,13 +85,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,69 +119,121 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s" s="1">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E2" t="n" s="0">
-        <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>7</v>
       </c>
       <c r="D3" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="E3" t="n" s="0">
+      <c r="E4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E5" t="n" s="0">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E6" t="n" s="0">
         <v>5.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="E7" t="n" s="0">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>